<commit_message>
18.04.19 Today 9:34AM Morning Updated
</commit_message>
<xml_diff>
--- a/Allocation Sheet.xlsx
+++ b/Allocation Sheet.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
   <si>
     <t>BL60</t>
   </si>
@@ -230,9 +230,6 @@
     <t>i95</t>
   </si>
   <si>
-    <t>i110</t>
-  </si>
-  <si>
     <t>L200</t>
   </si>
   <si>
@@ -296,7 +293,22 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>V75</t>
+    <t>i110_SKD</t>
+  </si>
+  <si>
+    <t>V75 SKD</t>
+  </si>
+  <si>
+    <t>Received By</t>
+  </si>
+  <si>
+    <t>DSR SIGN</t>
+  </si>
+  <si>
+    <t>Business Manager</t>
+  </si>
+  <si>
+    <t>Delivered By</t>
   </si>
 </sst>
 </file>
@@ -306,7 +318,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,6 +467,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -573,7 +597,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -689,28 +713,46 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 2" xfId="1"/>
@@ -720,6 +762,99 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>29158</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>9720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>11308</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Connector 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="29158" y="12547730"/>
+          <a:ext cx="1020536" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19439</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1039975</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>1588</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Connector 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6249567" y="12538010"/>
+          <a:ext cx="1020536" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1012,8 +1147,8 @@
   </sheetPr>
   <dimension ref="A1:S134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection sqref="A1:M60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="12.75"/>
@@ -1173,10 +1308,10 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="H6" s="20" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="I6" s="26">
-        <v>7890</v>
+        <v>7490</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="7"/>
@@ -1195,10 +1330,10 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="H7" s="21" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="I7" s="34">
-        <v>7490</v>
+        <v>8340</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="7"/>
@@ -1217,10 +1352,10 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="H8" s="35" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="I8" s="24">
-        <v>9240</v>
+        <v>9190</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="7"/>
@@ -1229,7 +1364,7 @@
     </row>
     <row r="9" spans="1:19" ht="16.5" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="32">
         <v>800</v>
@@ -1239,10 +1374,10 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="H9" s="35" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I9" s="26">
-        <v>9190</v>
+        <v>3560</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="7"/>
@@ -1261,10 +1396,10 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="H10" s="21" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="I10" s="26">
-        <v>3560</v>
+        <v>3340</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="7"/>
@@ -1283,10 +1418,10 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="H11" s="21" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="I11" s="26">
-        <v>3340</v>
+        <v>4690</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="7"/>
@@ -1305,10 +1440,10 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="H12" s="22" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="I12" s="26">
-        <v>4690</v>
+        <v>5390</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="7"/>
@@ -1317,7 +1452,7 @@
     </row>
     <row r="13" spans="1:19" ht="16.5" customHeight="1">
       <c r="A13" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="32">
         <v>910</v>
@@ -1327,10 +1462,10 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="H13" s="20" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="I13" s="26">
-        <v>5390</v>
+        <v>4970</v>
       </c>
       <c r="J13" s="12"/>
       <c r="K13" s="7"/>
@@ -1349,10 +1484,10 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="H14" s="22" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="I14" s="26">
-        <v>4970</v>
+        <v>3710</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="7"/>
@@ -1371,10 +1506,10 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="H15" s="20" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="I15" s="26">
-        <v>3880</v>
+        <v>3620</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="7"/>
@@ -1393,10 +1528,10 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="H16" s="20" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="I16" s="26">
-        <v>3999</v>
+        <v>4620</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="7"/>
@@ -1405,7 +1540,7 @@
     </row>
     <row r="17" spans="1:13" ht="16.5" customHeight="1">
       <c r="A17" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" s="32">
         <v>1010</v>
@@ -1415,10 +1550,10 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="H17" s="35" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="I17" s="26">
-        <v>4620</v>
+        <v>4520</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="7"/>
@@ -1437,10 +1572,10 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="H18" s="35" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="I18" s="26">
-        <v>4520</v>
+        <v>4080</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="7"/>
@@ -1459,10 +1594,10 @@
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="H19" s="20" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="I19" s="26">
-        <v>4270</v>
+        <v>4360</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="7"/>
@@ -1481,10 +1616,10 @@
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="H20" s="35" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="I20" s="26">
-        <v>4360</v>
+        <v>4640</v>
       </c>
       <c r="J20" s="12"/>
       <c r="K20" s="7"/>
@@ -1493,20 +1628,20 @@
     </row>
     <row r="21" spans="1:13" ht="16.5" customHeight="1">
       <c r="A21" s="22" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="B21" s="32">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="H21" s="35" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I21" s="26">
-        <v>4360</v>
+        <v>5650</v>
       </c>
       <c r="J21" s="12"/>
       <c r="K21" s="7"/>
@@ -1515,20 +1650,20 @@
     </row>
     <row r="22" spans="1:13" ht="16.5" customHeight="1">
       <c r="A22" s="22" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B22" s="32">
-        <v>1000</v>
+        <v>960</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="H22" s="35" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="I22" s="26">
-        <v>4840</v>
+        <v>5020</v>
       </c>
       <c r="J22" s="12"/>
       <c r="K22" s="7"/>
@@ -1537,20 +1672,20 @@
     </row>
     <row r="23" spans="1:13" ht="16.5" customHeight="1">
       <c r="A23" s="22" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B23" s="32">
-        <v>960</v>
+        <v>980</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="H23" s="35" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I23" s="26">
-        <v>5650</v>
+        <v>5280</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="7"/>
@@ -1559,20 +1694,20 @@
     </row>
     <row r="24" spans="1:13" ht="16.5" customHeight="1">
       <c r="A24" s="22" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B24" s="32">
-        <v>980</v>
+        <v>1040</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="H24" s="35" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="I24" s="26">
-        <v>5020</v>
+        <v>5440</v>
       </c>
       <c r="J24" s="12"/>
       <c r="K24" s="7"/>
@@ -1581,20 +1716,20 @@
     </row>
     <row r="25" spans="1:13" ht="16.5" customHeight="1">
       <c r="A25" s="22" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B25" s="32">
-        <v>1040</v>
+        <v>1290</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="H25" s="35" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="I25" s="26">
-        <v>5280</v>
+        <v>5560</v>
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="7"/>
@@ -1603,20 +1738,20 @@
     </row>
     <row r="26" spans="1:13" ht="16.5" customHeight="1">
       <c r="A26" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B26" s="32">
-        <v>1290</v>
+        <v>1270</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="H26" s="35" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="I26" s="26">
-        <v>5440</v>
+        <v>6090</v>
       </c>
       <c r="J26" s="12"/>
       <c r="K26" s="7"/>
@@ -1625,20 +1760,20 @@
     </row>
     <row r="27" spans="1:13" ht="16.5" customHeight="1">
       <c r="A27" s="22" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="B27" s="32">
-        <v>1270</v>
+        <v>1190</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="H27" s="21" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I27" s="26">
-        <v>5560</v>
+        <v>5390</v>
       </c>
       <c r="J27" s="12"/>
       <c r="K27" s="7"/>
@@ -1647,20 +1782,20 @@
     </row>
     <row r="28" spans="1:13" ht="16.5" customHeight="1">
       <c r="A28" s="22" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="B28" s="32">
-        <v>1190</v>
+        <v>1290</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="H28" s="21" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="I28" s="26">
-        <v>6090</v>
+        <v>12590</v>
       </c>
       <c r="J28" s="12"/>
       <c r="K28" s="7"/>
@@ -1669,20 +1804,20 @@
     </row>
     <row r="29" spans="1:13" ht="16.5" customHeight="1">
       <c r="A29" s="22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B29" s="32">
-        <v>1290</v>
+        <v>1190</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="H29" s="22" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="I29" s="34">
-        <v>5390</v>
+        <v>12240</v>
       </c>
       <c r="J29" s="12"/>
       <c r="K29" s="7"/>
@@ -1691,20 +1826,20 @@
     </row>
     <row r="30" spans="1:13" ht="16.5" customHeight="1">
       <c r="A30" s="22" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="B30" s="32">
-        <v>1190</v>
+        <v>1080</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="H30" s="20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I30" s="34">
-        <v>12590</v>
+        <v>12090</v>
       </c>
       <c r="J30" s="12"/>
       <c r="K30" s="7"/>
@@ -1713,20 +1848,20 @@
     </row>
     <row r="31" spans="1:13" ht="16.5" customHeight="1">
       <c r="A31" s="22" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B31" s="32">
-        <v>1080</v>
+        <v>1100</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="H31" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I31" s="34">
-        <v>12240</v>
+        <v>10840</v>
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="7"/>
@@ -1735,20 +1870,20 @@
     </row>
     <row r="32" spans="1:13" ht="16.5" customHeight="1">
       <c r="A32" s="22" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B32" s="32">
-        <v>1100</v>
+        <v>1120</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="H32" s="20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I32" s="26">
-        <v>12090</v>
+        <v>12490</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="7"/>
@@ -1757,20 +1892,20 @@
     </row>
     <row r="33" spans="1:13" ht="16.5" customHeight="1">
       <c r="A33" s="22" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B33" s="32">
-        <v>1120</v>
+        <v>1040</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="H33" s="22" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I33" s="34">
-        <v>10840</v>
+        <v>12800</v>
       </c>
       <c r="J33" s="12"/>
       <c r="K33" s="7"/>
@@ -1779,20 +1914,20 @@
     </row>
     <row r="34" spans="1:13" ht="16.5" customHeight="1">
       <c r="A34" s="22" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B34" s="32">
-        <v>1040</v>
+        <v>1100</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="H34" s="35" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I34" s="26">
-        <v>12490</v>
+        <v>17790</v>
       </c>
       <c r="J34" s="12"/>
       <c r="K34" s="7"/>
@@ -1801,7 +1936,7 @@
     </row>
     <row r="35" spans="1:13" ht="16.5" customHeight="1">
       <c r="A35" s="22" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="B35" s="33">
         <v>1100</v>
@@ -1811,10 +1946,10 @@
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="H35" s="20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I35" s="26">
-        <v>12800</v>
+        <v>7740</v>
       </c>
       <c r="J35" s="12"/>
       <c r="K35" s="7"/>
@@ -1823,17 +1958,17 @@
     </row>
     <row r="36" spans="1:13" ht="16.5" customHeight="1">
       <c r="A36" s="22" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B36" s="32">
-        <v>1100</v>
+        <v>1130</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="H36" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I36" s="26">
         <v>17790</v>
@@ -1845,17 +1980,17 @@
     </row>
     <row r="37" spans="1:13" ht="16.5" customHeight="1">
       <c r="A37" s="22" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B37" s="32">
-        <v>1130</v>
+        <v>1100</v>
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="H37" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I37" s="26">
         <v>7740</v>
@@ -1867,10 +2002,10 @@
     </row>
     <row r="38" spans="1:13" ht="16.5" customHeight="1">
       <c r="A38" s="22" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B38" s="32">
-        <v>1100</v>
+        <v>1330</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="7"/>
@@ -1885,7 +2020,7 @@
     </row>
     <row r="39" spans="1:13" ht="16.5" customHeight="1">
       <c r="A39" s="22" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="B39" s="32">
         <v>1330</v>
@@ -1903,10 +2038,10 @@
     </row>
     <row r="40" spans="1:13" ht="16.5" customHeight="1">
       <c r="A40" s="22" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B40" s="32">
-        <v>1330</v>
+        <v>1200</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="7"/>
@@ -1921,10 +2056,10 @@
     </row>
     <row r="41" spans="1:13" ht="16.5" customHeight="1">
       <c r="A41" s="22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B41" s="32">
-        <v>1200</v>
+        <v>1220</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="7"/>
@@ -1939,10 +2074,10 @@
     </row>
     <row r="42" spans="1:13" ht="16.5" customHeight="1">
       <c r="A42" s="22" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="B42" s="32">
-        <v>1220</v>
+        <v>1460</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="7"/>
@@ -1960,89 +2095,89 @@
         <v>78</v>
       </c>
       <c r="B43" s="32">
-        <v>1460</v>
+        <v>1470</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
-      <c r="H43" s="45" t="s">
+      <c r="H43" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="I43" s="52"/>
+      <c r="I43" s="50"/>
       <c r="J43" s="37"/>
-      <c r="K43" s="45"/>
-      <c r="L43" s="46"/>
+      <c r="K43" s="49"/>
+      <c r="L43" s="51"/>
       <c r="M43" s="17"/>
     </row>
     <row r="44" spans="1:13" ht="16.5" customHeight="1">
       <c r="A44" s="22" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B44" s="32">
-        <v>1470</v>
+        <v>1590</v>
       </c>
       <c r="C44" s="12"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="51"/>
-      <c r="J44" s="51"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51"/>
-      <c r="M44" s="46"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="52"/>
+      <c r="L44" s="52"/>
+      <c r="M44" s="51"/>
     </row>
     <row r="45" spans="1:13" ht="16.5" customHeight="1">
       <c r="A45" s="22" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B45" s="32">
-        <v>1590</v>
+        <v>1480</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
-      <c r="H45" s="47" t="s">
+      <c r="H45" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="I45" s="47"/>
-      <c r="J45" s="47"/>
-      <c r="K45" s="47"/>
-      <c r="L45" s="47"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="45"/>
+      <c r="L45" s="45"/>
       <c r="M45" s="44"/>
     </row>
     <row r="46" spans="1:13" ht="16.5" customHeight="1">
       <c r="A46" s="22" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="B46" s="32">
-        <v>1480</v>
+        <v>1730</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
       <c r="H46" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I46" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="J46" s="48" t="s">
+      <c r="J46" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="K46" s="49"/>
-      <c r="L46" s="50"/>
+      <c r="K46" s="47"/>
+      <c r="L46" s="48"/>
       <c r="M46" s="44"/>
     </row>
     <row r="47" spans="1:13" ht="16.5" customHeight="1">
       <c r="A47" s="22" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B47" s="32">
-        <v>1730</v>
+        <v>1250</v>
       </c>
       <c r="C47" s="12"/>
       <c r="D47" s="7"/>
@@ -2059,10 +2194,10 @@
     </row>
     <row r="48" spans="1:13" ht="16.5" customHeight="1">
       <c r="A48" s="22" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B48" s="32">
-        <v>1250</v>
+        <v>1370</v>
       </c>
       <c r="C48" s="12"/>
       <c r="D48" s="7"/>
@@ -2079,10 +2214,10 @@
     </row>
     <row r="49" spans="1:13" ht="16.5" customHeight="1">
       <c r="A49" s="25" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B49" s="25">
-        <v>1370</v>
+        <v>1890</v>
       </c>
       <c r="C49" s="12"/>
       <c r="D49" s="7"/>
@@ -2099,10 +2234,10 @@
     </row>
     <row r="50" spans="1:13" ht="16.5" customHeight="1">
       <c r="A50" s="25" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B50" s="25">
-        <v>1890</v>
+        <v>2780</v>
       </c>
       <c r="C50" s="12"/>
       <c r="D50" s="7"/>
@@ -2119,10 +2254,10 @@
     </row>
     <row r="51" spans="1:13" ht="16.5" customHeight="1">
       <c r="A51" s="25" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B51" s="25">
-        <v>2860</v>
+        <v>6540</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="7"/>
@@ -2139,10 +2274,10 @@
     </row>
     <row r="52" spans="1:13" ht="16.5" customHeight="1">
       <c r="A52" s="25" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B52" s="25">
-        <v>6540</v>
+        <v>6210</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="7"/>
@@ -2159,10 +2294,10 @@
     </row>
     <row r="53" spans="1:13" ht="16.5" customHeight="1">
       <c r="A53" s="25" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="B53" s="25">
-        <v>6210</v>
+        <v>7075</v>
       </c>
       <c r="C53" s="12"/>
       <c r="D53" s="7"/>
@@ -2179,10 +2314,10 @@
     </row>
     <row r="54" spans="1:13" ht="16.5" customHeight="1">
       <c r="A54" s="25" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B54" s="25">
-        <v>7075</v>
+        <v>7910</v>
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="7"/>
@@ -2199,10 +2334,10 @@
     </row>
     <row r="55" spans="1:13" ht="16.5" customHeight="1">
       <c r="A55" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B55" s="24">
-        <v>7910</v>
+        <v>7890</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="18"/>
@@ -2220,10 +2355,34 @@
     <row r="56" spans="1:13" ht="16.5" customHeight="1">
       <c r="M56" s="36"/>
     </row>
-    <row r="57" spans="1:13" ht="16.5" customHeight="1"/>
-    <row r="58" spans="1:13" ht="16.5" customHeight="1"/>
-    <row r="59" spans="1:13" ht="16.5" customHeight="1"/>
-    <row r="60" spans="1:13" ht="16.5" customHeight="1"/>
+    <row r="57" spans="1:13" ht="16.5" customHeight="1">
+      <c r="A57" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="53"/>
+      <c r="M57" s="58" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="16.5" customHeight="1">
+      <c r="A58" s="53"/>
+      <c r="B58" s="53"/>
+      <c r="M58" s="55"/>
+    </row>
+    <row r="59" spans="1:13" ht="16.5" customHeight="1">
+      <c r="A59" s="53"/>
+      <c r="B59" s="53"/>
+      <c r="M59" s="55"/>
+    </row>
+    <row r="60" spans="1:13" ht="16.5" customHeight="1">
+      <c r="A60" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B60" s="57"/>
+      <c r="M60" s="56" t="s">
+        <v>95</v>
+      </c>
+    </row>
     <row r="61" spans="1:13" ht="16.5" customHeight="1"/>
     <row r="62" spans="1:13" ht="16.5" customHeight="1">
       <c r="G62" s="16"/>
@@ -2303,7 +2462,11 @@
     <row r="133" ht="15" customHeight="1"/>
     <row r="134" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B59"/>
+    <mergeCell ref="M58:M59"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:M3"/>
@@ -2317,6 +2480,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="89" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="83" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>